<commit_message>
New changes - 6/30/2020
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anand\Development\KasTech\AR2.0\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Documents\UiPath\AR2.0\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FEFCA7-7C1F-4070-89E6-40B728B19A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -90,19 +89,7 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -124,13 +111,31 @@
     <t>MappingFilePath</t>
   </si>
   <si>
-    <t>D:\Anand\Development\KasTech\AR2.0\Data\MappingSheet.xlsx</t>
+    <t>C:\Users\Hp\Documents\UiPath\AR2.0\Data\MappingSheet.xlsx</t>
+  </si>
+  <si>
+    <t>MappingFilePath_BankReport_SheetName</t>
+  </si>
+  <si>
+    <t>Bank_Report</t>
+  </si>
+  <si>
+    <t>MappingFilePath_RemittanceReport_SheetName</t>
+  </si>
+  <si>
+    <t>Remittance_Report</t>
+  </si>
+  <si>
+    <t>PNC_BankReport_SheetName</t>
+  </si>
+  <si>
+    <t>Bank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -177,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -186,6 +191,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,11 +508,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -549,39 +557,50 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:26" ht="30">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
         <v>32</v>
       </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
     </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1568,10 +1587,6 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1580,10 +1595,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z987"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z985"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1631,81 +1648,81 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2681,8 +2698,6 @@
     <row r="983" ht="14.25" customHeight="1"/>
     <row r="984" ht="14.25" customHeight="1"/>
     <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2690,7 +2705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
updated code except Aggregation logic
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -15,13 +15,14 @@
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
+    <sheet name="BankMappingSheet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -108,12 +109,6 @@
     <t>Static part of logging message. Calling Get Transaction Data.</t>
   </si>
   <si>
-    <t>MappingFilePath</t>
-  </si>
-  <si>
-    <t>C:\Users\Hp\Documents\UiPath\AR2.0\Data\MappingSheet.xlsx</t>
-  </si>
-  <si>
     <t>MappingFilePath_BankReport_SheetName</t>
   </si>
   <si>
@@ -130,13 +125,64 @@
   </si>
   <si>
     <t>Bank</t>
+  </si>
+  <si>
+    <t>BankReport_TableName</t>
+  </si>
+  <si>
+    <t>RPA_AR_BANK_REPORTS_TBL</t>
+  </si>
+  <si>
+    <t>CompanyReport_TableName</t>
+  </si>
+  <si>
+    <t>RPA_AR_REMITTANCE_TBL</t>
+  </si>
+  <si>
+    <t>Bank Report</t>
+  </si>
+  <si>
+    <t>FileType</t>
+  </si>
+  <si>
+    <t>FolderPath</t>
+  </si>
+  <si>
+    <t>Bridge Bank</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>C:\Users\Hp\Documents\UiPath\AR2.0\Data\Input\BankReport\</t>
+  </si>
+  <si>
+    <t>PNC Bank</t>
+  </si>
+  <si>
+    <t>Customer_LookUp_Table</t>
+  </si>
+  <si>
+    <t>SELECT * FROM RPA_AR_REMIT_CUST_LOOKUP</t>
+  </si>
+  <si>
+    <t>DB_Connection_String</t>
+  </si>
+  <si>
+    <t>Data Source=tmw-dev-sql01.amerit.com;Initial Catalog=TMWAMS_RPA;Persist Security Info=True;User ID=RPA;Password=Welcome_2019</t>
+  </si>
+  <si>
+    <t>DB_Provider_Name</t>
+  </si>
+  <si>
+    <t>System.Data.SqlClient</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -161,16 +207,30 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -178,14 +238,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -195,6 +269,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,16 +586,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z991"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -564,15 +641,15 @@
       <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -600,10 +677,38 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1585,8 +1690,6 @@
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
     <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1648,10 +1751,10 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3755,4 +3858,55 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>